<commit_message>
Avances IPC_Supermarket and others
</commit_message>
<xml_diff>
--- a/data/Construcción IPC/outputs/categorias_subcategorias.xlsx
+++ b/data/Construcción IPC/outputs/categorias_subcategorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B167"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chocol. y Caramelos</t>
+          <t>Chocolates y Caramelos</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Chocolates y Caramelos</t>
+          <t>Comidas en Conserva</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Comidas en Conserva</t>
+          <t>Condimentos y Legumbres</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Condimentos y Legumbres</t>
+          <t>Dietéticos y Saludables</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dietéticos y Saludables</t>
+          <t>Frutas en Conserva</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Frutas en Conserva</t>
+          <t>Galletas</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Galletas</t>
+          <t>Golosinas - Varias</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Golosinas - Varias</t>
+          <t>Mascotas</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mascotas</t>
+          <t>Mermel, Mieles</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mermel, Mieles</t>
+          <t>Nutrición Infantil</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nutrición Infantil</t>
+          <t>Productos Americanos</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Productos Americanos</t>
+          <t>Productos Importados</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Productos Importados</t>
+          <t>Repostería</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Repostería</t>
+          <t>Salsas y Extracto de Tomate</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Salsas y Extracto de Tomate</t>
+          <t>Snack</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Snack</t>
+          <t>Temporada</t>
         </is>
       </c>
     </row>
@@ -681,19 +681,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Temporada</t>
+          <t>Verduras en Conserva</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Abarrotes</t>
+          <t>Aseo Del Bebé</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Verduras en Conserva</t>
+          <t>Aseo Del Bebé</t>
         </is>
       </c>
     </row>
@@ -705,19 +705,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Aseo Del Bebé</t>
+          <t>Pañales</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Aseo Del Bebé</t>
+          <t>Aseo Del Hogar</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pañales</t>
+          <t>Accesorios Del Hogar</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Accesorios Del Hogar</t>
+          <t>Limpieza De La Ropa</t>
         </is>
       </c>
     </row>
@@ -741,19 +741,19 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Limpieza De La Ropa</t>
+          <t>Limpieza De Living y Roperos</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Aseo Del Hogar</t>
+          <t>Aseo Personal</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Limpieza De Living y Roperos</t>
+          <t>Cuidado De La Piel</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cuidado De La Piel</t>
+          <t>Cuidado Del Cabello</t>
         </is>
       </c>
     </row>
@@ -777,19 +777,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cuidado Del Cabello</t>
+          <t>Cuidado Familiar</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Aseo Personal</t>
+          <t>Bazar</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cuidado Familiar</t>
+          <t>Articulos de Bebé</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Articulos de Bebé</t>
+          <t>Articulos de Cocina</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Articulos de Cocina</t>
+          <t>Automotriz</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Automotriz</t>
+          <t>Baño General</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Baño General</t>
+          <t>Bijouteria/Cuidado Personal</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bijouteria/Cuidado Personal</t>
+          <t>Bioseguridad</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bioseguridad</t>
+          <t>Bolsos/Carteras/Maletas</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Bolsos/Carteras/Maletas</t>
+          <t>Camping General</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Camping General</t>
+          <t>Churrasquería</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Churrasquería</t>
+          <t>Computadora/Cámara/Filmadora y Accesorio</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Computadora/Cámara/Filmadora y Accesorio</t>
+          <t>Cotillón</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cotillón</t>
+          <t>Electrodoméstico Cuidado Personal</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Electrodoméstico Cuidado Personal</t>
+          <t>Electrodoméstico Reproductores Sonido</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Electrodoméstico Reproductores Sonido</t>
+          <t>Electrodoméstico/Línea Blanca-Hogar</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Electrodoméstico/Línea Blanca-Hogar</t>
+          <t>Ferretería</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ferretería</t>
+          <t>Jardinería General</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Jardinería General</t>
+          <t>Librería</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Librería</t>
+          <t>Living y Dormitorio</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Living y Dormitorio</t>
+          <t>Mascotas General</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mascotas General</t>
+          <t>Menaje Metálico</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Menaje Metálico</t>
+          <t>Menaje Plástico</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Menaje Plástico</t>
+          <t>Menaje Porcelana/Cerámica</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Menaje Porcelana/Cerámica</t>
+          <t>Menaje Vidrio/Cristal</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Menaje Vidrio/Cristal</t>
+          <t>Regalos/Adornos</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Regalos/Adornos</t>
+          <t>Telefonía y Accesorios</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Telefonía y Accesorios</t>
+          <t>Temporada Carnaval</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Temporada Carnaval</t>
+          <t>Temporada Halloween</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Temporada Halloween</t>
+          <t>Temporada Navidad</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Temporada Navidad</t>
+          <t>Temporada Verano</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Temporada Verano</t>
+          <t>Temporadas Restantes</t>
         </is>
       </c>
     </row>
@@ -1149,19 +1149,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Temporadas Restantes</t>
+          <t>Textiles Genéricos/Temporadas</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Bazar</t>
+          <t>Bazar Importación</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Textiles Genéricos/Temporadas</t>
+          <t>Artículos para Bebé</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Artículos para Bebé</t>
+          <t>Baño General</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Baño General</t>
+          <t>Bijouteria/Cuidado Personal</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Bijouteria/Cuidado Personal</t>
+          <t>Camping General</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Camping General</t>
+          <t>Churrasquería</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Churrasquería</t>
+          <t>Cocina General</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cocina General</t>
+          <t>Computadoras/Camaras/Filma y  Accesorio</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Computadoras/Camaras/Filma y  Accesorio</t>
+          <t>Cotillón</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Cotillón</t>
+          <t>Diferenciales Usa</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Diferenciales Usa</t>
+          <t>Electrodomésticos Cuidado Personal</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Electrodomésticos Cuidado Personal</t>
+          <t>Ferretería</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Ferretería</t>
+          <t>Librería</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Librería</t>
+          <t>Living y Dormitorio</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Living y Dormitorio</t>
+          <t>Menaje Metálico</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Menaje Metálico</t>
+          <t>Menaje Plástico</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Menaje Plástico</t>
+          <t>Menaje Porcelana/Cerámica</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Menaje Porcelana/Cerámica</t>
+          <t>Menaje Vidrio/Cristal</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Menaje Vidrio/Cristal</t>
+          <t>Mueblería General</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Mueblería General</t>
+          <t>Regalos/Adornos</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Regalos/Adornos</t>
+          <t>Telefonia y Accesorios</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Telefonia y Accesorios</t>
+          <t>Temporada Carnaval</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Temporada Carnaval</t>
+          <t>Temporada Halloween</t>
         </is>
       </c>
     </row>
@@ -1425,19 +1425,19 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Temporada Halloween</t>
+          <t>Temporada Navidad</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Bazar Importación</t>
+          <t>Bebidas</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Temporada Navidad</t>
+          <t>Aguas</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Aguas</t>
+          <t>Bebidas Usa</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Bebidas Usa</t>
+          <t>Bebidas Varias</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Bebidas Varias</t>
+          <t>Cervezas</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Cervezas</t>
+          <t>Cigarrillos</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Cigarrillos</t>
+          <t>Energizantes</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Energizantes</t>
+          <t>Gaseosas</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Gaseosas</t>
+          <t>Hielos</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Hielos</t>
+          <t>Isotónicos</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Isotónicos</t>
+          <t>Jugos, Néctar</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Jugos, Néctar</t>
+          <t>Licores</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Licores</t>
+          <t>Refrescos en Polvo</t>
         </is>
       </c>
     </row>
@@ -1581,19 +1581,19 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Refrescos en Polvo</t>
+          <t>Vinos y Champagne</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Bebidas</t>
+          <t>Carnes</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Vinos y Champagne</t>
+          <t>Carne de Pollo</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Carne de Pollo</t>
+          <t>Carne de Res</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Carne de Res</t>
+          <t>Carnes Procesadas</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Carnes Procesadas</t>
+          <t>Carnes al Vacio Externas</t>
         </is>
       </c>
     </row>
@@ -1641,19 +1641,19 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Carnes al Vacio Externas</t>
+          <t>Otras Carnes</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Carnes</t>
+          <t>Congelados</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Otras Carnes</t>
+          <t>Carnes Congeladas</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Carnes Congeladas</t>
+          <t>Helados, Cassattas y Picoleses</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Helados, Cassattas y Picoleses</t>
+          <t>Masas y Comidas Congeladas</t>
         </is>
       </c>
     </row>
@@ -1689,19 +1689,19 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Masas y Comidas Congeladas</t>
+          <t>Pulpas y Frutas Congeladas</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Congelados</t>
+          <t>Cuidado Personal</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Pulpas y Frutas Congeladas</t>
+          <t>Cuidado Bucal</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Cuidado Bucal</t>
+          <t>Cuidado Familiar</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Cuidado Familiar</t>
+          <t>Cuidado de la Piel</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Cuidado de la Piel</t>
+          <t>Cuidado del Adulto</t>
         </is>
       </c>
     </row>
@@ -1749,19 +1749,19 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Cuidado del Adulto</t>
+          <t>Cuidado del Cabello</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Cuidado Personal</t>
+          <t>Cuidado del Bebé</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Cuidado del Cabello</t>
+          <t>Cuidado del Bebé</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Cuidado del Bebé</t>
+          <t>Kids</t>
         </is>
       </c>
     </row>
@@ -1785,19 +1785,19 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Kids</t>
+          <t>Pañales</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Cuidado del Bebé</t>
+          <t>Cuidado del Hogar</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Pañales</t>
+          <t>Accesorios del Hogar</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Accesorios del Hogar</t>
+          <t>Insecticidas</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Insecticidas</t>
+          <t>Limpieza de Baños</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Limpieza de Baños</t>
+          <t>Limpieza de Cocina</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Limpieza de Cocina</t>
+          <t>Limpieza de Living y Ropero</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Limpieza de Living y Ropero</t>
+          <t>Limpieza de Zapatos</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Limpieza de Zapatos</t>
+          <t>Limpieza de la Ropa</t>
         </is>
       </c>
     </row>
@@ -1881,19 +1881,19 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Limpieza de la Ropa</t>
+          <t>Productos Americanos</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Cuidado del Hogar</t>
+          <t>Farmacia Otc</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Productos Americanos</t>
+          <t>Artículos Bebé</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Artículos Bebé</t>
+          <t>Dermatológicos</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Dermatológicos</t>
+          <t>Sistema Nervioso Central</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Sistema Nervioso Central</t>
+          <t>Sistema Respiratorio</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Sistema Respiratorio</t>
+          <t>Tracto Alimentario y Metabolismo</t>
         </is>
       </c>
     </row>
@@ -1953,19 +1953,19 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Tracto Alimentario y Metabolismo</t>
+          <t>Varios</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Farmacia Otc</t>
+          <t>Farmacia Éticos</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Varios</t>
+          <t>Dermatológicos</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Dermatológicos</t>
+          <t>Sistema Respiratorio</t>
         </is>
       </c>
     </row>
@@ -1989,19 +1989,19 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Sistema Respiratorio</t>
+          <t>Tracto Alimentario y Metabolismo</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Farmacia Éticos</t>
+          <t>Fiambres</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Tracto Alimentario y Metabolismo</t>
+          <t>Fiambres Externos</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Fiambres Externos</t>
+          <t>Fiambres Hipermaxi</t>
         </is>
       </c>
     </row>
@@ -2025,19 +2025,19 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Fiambres Hipermaxi</t>
+          <t>Temporada San Juan Externos</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Fiambres</t>
+          <t>Frutas y Verduras</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Temporada San Juan Externos</t>
+          <t>Frutas</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Frutas</t>
+          <t>Gourmet</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Gourmet</t>
+          <t>Ofertas Especiales</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Ofertas Especiales</t>
+          <t>Temporada</t>
         </is>
       </c>
     </row>
@@ -2085,19 +2085,19 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Temporada</t>
+          <t>Verduras</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Frutas y Verduras</t>
+          <t>Granos y Hortalizas</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Verduras</t>
+          <t>Derivados Hipermaxi</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Derivados Hipermaxi</t>
+          <t>Fraccionados Hipermaxi</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Fraccionados Hipermaxi</t>
+          <t>Hortalizas Delifresh</t>
         </is>
       </c>
     </row>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Hortalizas Delifresh</t>
+          <t>Postres Delifresh</t>
         </is>
       </c>
     </row>
@@ -2145,19 +2145,19 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Postres Delifresh</t>
+          <t>Sandwiches Delifresh</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Granos y Hortalizas</t>
+          <t>Juguetería</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sandwiches Delifresh</t>
+          <t>Juguetería Didáctica/Temporada</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Juguetería Didáctica/Temporada</t>
+          <t>Juguetería Marcas</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Juguetería Marcas</t>
+          <t>Juguetería Niña/Bebé</t>
         </is>
       </c>
     </row>
@@ -2193,19 +2193,19 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Juguetería Niña/Bebé</t>
+          <t>Juguetería Niño/Bebé</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Juguetería</t>
+          <t>Juguetería Importación</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Juguetería Niño/Bebé</t>
+          <t>Jugueteria Marcas</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Jugueteria Marcas</t>
+          <t>Juguetería Didáctica/Temporada</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Juguetería Didáctica/Temporada</t>
+          <t>Juguetería Niña/Bebé</t>
         </is>
       </c>
     </row>
@@ -2241,19 +2241,19 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Juguetería Niña/Bebé</t>
+          <t>Juguetería Niño/Bebé</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Juguetería Importación</t>
+          <t>Lácteos y Derivados</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Juguetería Niño/Bebé</t>
+          <t>Crema de Leche</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Crema de Leche</t>
+          <t>Dulces de Leche y Manjares</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Dulces de Leche y Manjares</t>
+          <t>Huevos</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Huevos</t>
+          <t>Leches</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Leches</t>
+          <t>Mantequillas y Margarinas</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Mantequillas y Margarinas</t>
+          <t>Postres</t>
         </is>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Postres</t>
+          <t>Quesos</t>
         </is>
       </c>
     </row>
@@ -2337,19 +2337,19 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Quesos</t>
+          <t>Yogures</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Lácteos y Derivados</t>
+          <t>Panadería</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Yogures</t>
+          <t>Panadería Especialidades Hipermaxi</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Panadería Especialidades Hipermaxi</t>
+          <t>Panadería Externa</t>
         </is>
       </c>
     </row>
@@ -2373,19 +2373,19 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Panadería Externa</t>
+          <t>Panadería Hipermaxi</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Panadería</t>
+          <t>Pastelería y Masas Típicas</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Panadería Hipermaxi</t>
+          <t>Masas Típicas Externas</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Masas Típicas Externas</t>
+          <t>Masas Típicas Hipermaxi</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Masas Típicas Hipermaxi</t>
+          <t>Pastelería Externa</t>
         </is>
       </c>
     </row>
@@ -2420,18 +2420,6 @@
         </is>
       </c>
       <c r="B166" t="inlineStr">
-        <is>
-          <t>Pastelería Externa</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Pastelería y Masas Típicas</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
         <is>
           <t>Pastelería Hipermaxi</t>
         </is>

</xml_diff>